<commit_message>
Ajout de la correction du sprint2 par le fichier Equipe207.xlsx
</commit_message>
<xml_diff>
--- a/Equipe207.xlsx
+++ b/Equipe207.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="254" documentId="8_{6BB8C8F4-817F-4135-A9EF-0E7E368F1CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65732D47-656B-4077-BE80-31274F7B8AAC}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="8_{6BB8C8F4-817F-4135-A9EF-0E7E368F1CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E52C952-C24D-4AC2-9719-58726C217389}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="9" r:id="rId1"/>
@@ -368,8 +368,8 @@
     <t>Il n'y a pas de duplication de code.</t>
   </si>
   <si>
-    <t>server\app\gateway\game\game.gateway.spec.ts [5:1 - 11:12] (6 lines, 97 tokens)
-server\app\gateway\join\join.gateway.spec.ts [1:1 - 7:12]
+    <t>server\app\gateway\game\game.gateway.ts [69:32 - 74:26] (5 lines, 104 tokens)
+server\app\gateway\game\game.gateway.ts [60:24 - 65:18]
 client\src\app\pages\host-game-page\host-game-page.component.ts [54:2 - 60:5] (6 lines, 74 tokens)
 client\src\app\pages\waiting-page\waiting-page.component.ts [60:7 - 66:2]
 client\src\app\events\game.events.ts [1:1 - 16:16] (15 lines, 121 tokens)
@@ -2363,6 +2363,102 @@
     <xf numFmtId="0" fontId="14" fillId="19" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="8" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="8" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="9" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="9" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="10" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="10" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="10" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2387,104 +2483,8 @@
     <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="8" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="8" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="8" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="9" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="9" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="9" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="10" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="10" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="10" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3062,8 +3062,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="B44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3082,36 +3082,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A2" s="231" t="s">
+      <c r="A2" s="263" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="231"/>
-      <c r="C2" s="231"/>
-      <c r="D2" s="231"/>
-      <c r="E2" s="231"/>
-      <c r="F2" s="231"/>
-      <c r="G2" s="231"/>
-      <c r="H2" s="231"/>
-      <c r="I2" s="231"/>
-      <c r="J2" s="231"/>
-      <c r="K2" s="231"/>
+      <c r="B2" s="263"/>
+      <c r="C2" s="263"/>
+      <c r="D2" s="263"/>
+      <c r="E2" s="263"/>
+      <c r="F2" s="263"/>
+      <c r="G2" s="263"/>
+      <c r="H2" s="263"/>
+      <c r="I2" s="263"/>
+      <c r="J2" s="263"/>
+      <c r="K2" s="263"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
     <row r="4" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A4" s="232" t="s">
+      <c r="A4" s="264" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="232"/>
-      <c r="C4" s="232"/>
-      <c r="D4" s="232"/>
-      <c r="E4" s="232"/>
-      <c r="F4" s="232"/>
-      <c r="G4" s="232"/>
-      <c r="H4" s="232"/>
-      <c r="I4" s="232"/>
-      <c r="J4" s="232"/>
-      <c r="K4" s="232"/>
+      <c r="B4" s="264"/>
+      <c r="C4" s="264"/>
+      <c r="D4" s="264"/>
+      <c r="E4" s="264"/>
+      <c r="F4" s="264"/>
+      <c r="G4" s="264"/>
+      <c r="H4" s="264"/>
+      <c r="I4" s="264"/>
+      <c r="J4" s="264"/>
+      <c r="K4" s="264"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
@@ -3131,36 +3131,36 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A6" s="249" t="s">
+      <c r="A6" s="256" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="236" t="s">
+      <c r="B6" s="268" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="251" t="s">
+      <c r="C6" s="258" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="252"/>
-      <c r="E6" s="252"/>
-      <c r="F6" s="253" t="s">
+      <c r="D6" s="259"/>
+      <c r="E6" s="259"/>
+      <c r="F6" s="260" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="254"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="233" t="s">
+      <c r="G6" s="261"/>
+      <c r="H6" s="262"/>
+      <c r="I6" s="265" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="234"/>
-      <c r="K6" s="235"/>
+      <c r="J6" s="266"/>
+      <c r="K6" s="267"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="247"/>
-      <c r="O6" s="248"/>
-      <c r="P6" s="248"/>
+      <c r="N6" s="254"/>
+      <c r="O6" s="255"/>
+      <c r="P6" s="255"/>
     </row>
     <row r="7" spans="1:17" ht="18.75">
-      <c r="A7" s="250"/>
-      <c r="B7" s="237"/>
+      <c r="A7" s="257"/>
+      <c r="B7" s="269"/>
       <c r="C7" s="14" t="s">
         <v>15</v>
       </c>
@@ -3196,28 +3196,28 @@
       <c r="Q7" s="40"/>
     </row>
     <row r="8" spans="1:17" ht="18.75">
-      <c r="A8" s="246" t="s">
+      <c r="A8" s="238" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="246"/>
-      <c r="C8" s="239" t="s">
+      <c r="B8" s="238"/>
+      <c r="C8" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="240"/>
+      <c r="D8" s="232"/>
       <c r="E8" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="239" t="s">
+      <c r="F8" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="240"/>
+      <c r="G8" s="232"/>
       <c r="H8" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="239" t="s">
+      <c r="I8" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="240"/>
+      <c r="J8" s="232"/>
       <c r="K8" s="46"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -3305,10 +3305,10 @@
       <c r="Q10" s="40"/>
     </row>
     <row r="11" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A11" s="241" t="s">
+      <c r="A11" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="242"/>
+      <c r="B11" s="234"/>
       <c r="C11" s="47">
         <f>SUMPRODUCT(C6:C10,D6:D10)</f>
         <v>8</v>
@@ -3344,28 +3344,28 @@
       <c r="Q11" s="44"/>
     </row>
     <row r="12" spans="1:17" s="12" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A12" s="246" t="s">
+      <c r="A12" s="238" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="246"/>
-      <c r="C12" s="239" t="s">
+      <c r="B12" s="238"/>
+      <c r="C12" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="240"/>
+      <c r="D12" s="232"/>
       <c r="E12" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="239" t="s">
+      <c r="F12" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="240"/>
+      <c r="G12" s="232"/>
       <c r="H12" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="239" t="s">
+      <c r="I12" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="240"/>
+      <c r="J12" s="232"/>
       <c r="K12" s="46"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -3560,10 +3560,10 @@
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A18" s="241" t="s">
+      <c r="A18" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="242"/>
+      <c r="B18" s="234"/>
       <c r="C18" s="47">
         <f>SUMPRODUCT(C13:C17,D13:D17)</f>
         <v>13.8</v>
@@ -3599,28 +3599,28 @@
       <c r="Q18" s="44"/>
     </row>
     <row r="19" spans="1:17" s="43" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A19" s="238" t="s">
+      <c r="A19" s="270" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="238"/>
-      <c r="C19" s="239" t="s">
+      <c r="B19" s="270"/>
+      <c r="C19" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="240"/>
+      <c r="D19" s="232"/>
       <c r="E19" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="239" t="s">
+      <c r="F19" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="240"/>
+      <c r="G19" s="232"/>
       <c r="H19" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="239" t="s">
+      <c r="I19" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="240"/>
+      <c r="J19" s="232"/>
       <c r="K19" s="46"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
@@ -3696,10 +3696,10 @@
       <c r="M21" s="5"/>
     </row>
     <row r="22" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A22" s="243" t="s">
+      <c r="A22" s="271" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="244"/>
+      <c r="B22" s="253"/>
       <c r="C22" s="57">
         <f>SUMPRODUCT(C20:C21,D20:D21)</f>
         <v>6</v>
@@ -3735,24 +3735,24 @@
         <v>48</v>
       </c>
       <c r="B23" s="213"/>
-      <c r="C23" s="239" t="s">
+      <c r="C23" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="240"/>
+      <c r="D23" s="232"/>
       <c r="E23" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="239" t="s">
+      <c r="F23" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="240"/>
+      <c r="G23" s="232"/>
       <c r="H23" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="I23" s="239" t="s">
+      <c r="I23" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="240"/>
+      <c r="J23" s="232"/>
       <c r="K23" s="46"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -3855,10 +3855,10 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A27" s="245" t="s">
+      <c r="A27" s="252" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="244"/>
+      <c r="B27" s="253"/>
       <c r="C27" s="47">
         <f>SUMPRODUCT(C24:C26,D24:D26)</f>
         <v>2</v>
@@ -3890,28 +3890,28 @@
       <c r="M27" s="56"/>
     </row>
     <row r="28" spans="1:17" ht="21" customHeight="1">
-      <c r="A28" s="238" t="s">
+      <c r="A28" s="270" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="238"/>
-      <c r="C28" s="239" t="s">
+      <c r="B28" s="270"/>
+      <c r="C28" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="240"/>
+      <c r="D28" s="232"/>
       <c r="E28" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="F28" s="239" t="s">
+      <c r="F28" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="240"/>
+      <c r="G28" s="232"/>
       <c r="H28" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="I28" s="239" t="s">
+      <c r="I28" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="J28" s="240"/>
+      <c r="J28" s="232"/>
       <c r="K28" s="46"/>
       <c r="L28" s="9"/>
       <c r="M28" s="4"/>
@@ -4020,10 +4020,10 @@
       <c r="M31" s="5"/>
     </row>
     <row r="32" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A32" s="241" t="s">
+      <c r="A32" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="242"/>
+      <c r="B32" s="234"/>
       <c r="C32" s="47">
         <f>SUMPRODUCT(C29:C31,D29:D31)</f>
         <v>6</v>
@@ -4055,21 +4055,21 @@
       <c r="M32" s="56"/>
     </row>
     <row r="33" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A33" s="246" t="s">
+      <c r="A33" s="238" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="246"/>
-      <c r="C33" s="239" t="s">
+      <c r="B33" s="238"/>
+      <c r="C33" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="240"/>
+      <c r="D33" s="232"/>
       <c r="E33" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F33" s="239" t="s">
+      <c r="F33" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="G33" s="240"/>
+      <c r="G33" s="232"/>
       <c r="H33" s="46" t="s">
         <v>49</v>
       </c>
@@ -4218,10 +4218,10 @@
       <c r="M37" s="5"/>
     </row>
     <row r="38" spans="1:13" s="44" customFormat="1" ht="15.75">
-      <c r="A38" s="241" t="s">
+      <c r="A38" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="242"/>
+      <c r="B38" s="234"/>
       <c r="C38" s="69">
         <f>SUMPRODUCT(C34:C37,D34:D37)</f>
         <v>3.5</v>
@@ -4257,24 +4257,24 @@
         <v>82</v>
       </c>
       <c r="B39" s="45"/>
-      <c r="C39" s="239" t="s">
+      <c r="C39" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="240"/>
+      <c r="D39" s="232"/>
       <c r="E39" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="F39" s="239" t="s">
+      <c r="F39" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="G39" s="240"/>
+      <c r="G39" s="232"/>
       <c r="H39" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="I39" s="239" t="s">
+      <c r="I39" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="J39" s="240"/>
+      <c r="J39" s="232"/>
       <c r="K39" s="46"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
@@ -4612,10 +4612,10 @@
       <c r="M48" s="5"/>
     </row>
     <row r="49" spans="1:17" s="30" customFormat="1" ht="15.75">
-      <c r="A49" s="241" t="s">
+      <c r="A49" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="B49" s="242"/>
+      <c r="B49" s="234"/>
       <c r="C49" s="71">
         <f>SUMPRODUCT(C40:C48,D40:D48)</f>
         <v>40</v>
@@ -4651,28 +4651,28 @@
       <c r="Q49" s="44"/>
     </row>
     <row r="50" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A50" s="246" t="s">
+      <c r="A50" s="238" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="246"/>
-      <c r="C50" s="239" t="s">
+      <c r="B50" s="238"/>
+      <c r="C50" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="D50" s="240"/>
+      <c r="D50" s="232"/>
       <c r="E50" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="F50" s="239" t="s">
+      <c r="F50" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="G50" s="240"/>
+      <c r="G50" s="232"/>
       <c r="H50" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="I50" s="239" t="s">
+      <c r="I50" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="J50" s="240"/>
+      <c r="J50" s="232"/>
       <c r="K50" s="46"/>
       <c r="L50" s="8"/>
       <c r="M50" s="4"/>
@@ -4841,10 +4841,10 @@
       <c r="M55" s="5"/>
     </row>
     <row r="56" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A56" s="241" t="s">
+      <c r="A56" s="233" t="s">
         <v>27</v>
       </c>
-      <c r="B56" s="242"/>
+      <c r="B56" s="234"/>
       <c r="C56" s="57">
         <f>SUMPRODUCT(C51:C55,D51:D55)</f>
         <v>9.5</v>
@@ -4876,27 +4876,27 @@
       <c r="M56" s="56"/>
     </row>
     <row r="57" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A57" s="269" t="s">
+      <c r="A57" s="235" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="270"/>
-      <c r="C57" s="270"/>
-      <c r="D57" s="270"/>
-      <c r="E57" s="270"/>
-      <c r="F57" s="270"/>
-      <c r="G57" s="270"/>
-      <c r="H57" s="270"/>
-      <c r="I57" s="270"/>
-      <c r="J57" s="270"/>
-      <c r="K57" s="271"/>
+      <c r="B57" s="236"/>
+      <c r="C57" s="236"/>
+      <c r="D57" s="236"/>
+      <c r="E57" s="236"/>
+      <c r="F57" s="236"/>
+      <c r="G57" s="236"/>
+      <c r="H57" s="236"/>
+      <c r="I57" s="236"/>
+      <c r="J57" s="236"/>
+      <c r="K57" s="237"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
     </row>
     <row r="58" spans="1:17">
-      <c r="A58" s="256" t="s">
+      <c r="A58" s="239" t="s">
         <v>119</v>
       </c>
-      <c r="B58" s="257"/>
+      <c r="B58" s="240"/>
       <c r="C58" s="34">
         <f>C11+C18+C22+C27+C32+C38+C49+C56</f>
         <v>88.8</v>
@@ -4928,52 +4928,49 @@
       <c r="M58" s="5"/>
     </row>
     <row r="59" spans="1:17" s="44" customFormat="1" ht="15.75">
-      <c r="A59" s="258" t="s">
+      <c r="A59" s="241" t="s">
         <v>120</v>
       </c>
-      <c r="B59" s="259"/>
-      <c r="C59" s="260">
+      <c r="B59" s="242"/>
+      <c r="C59" s="243">
         <f>C58/D58</f>
         <v>0.88800000000000001</v>
       </c>
-      <c r="D59" s="261"/>
-      <c r="E59" s="262"/>
-      <c r="F59" s="263">
+      <c r="D59" s="244"/>
+      <c r="E59" s="245"/>
+      <c r="F59" s="246">
         <f>F58/G58</f>
         <v>0.78</v>
       </c>
-      <c r="G59" s="264"/>
-      <c r="H59" s="265"/>
-      <c r="I59" s="266">
+      <c r="G59" s="247"/>
+      <c r="H59" s="248"/>
+      <c r="I59" s="249">
         <f>I58/J58</f>
         <v>0</v>
       </c>
-      <c r="J59" s="267"/>
-      <c r="K59" s="268"/>
+      <c r="J59" s="250"/>
+      <c r="K59" s="251"/>
       <c r="L59" s="72"/>
       <c r="M59" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="I59:K59"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="N6:P6"/>
@@ -4990,22 +4987,25 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="I59:K59"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A56:B56"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L18 L22 L27 L32 L38 L49 L11 C9:C10 F9:F10 I9:I10 C24:C26 F24:F26 I24:I26 C34:C37 F34:F37 I34:I37 C51:C55 F51:F55 I51:I55 I13:I17 F13:F17 C13:C17 I20:I21 F20:F21 C20:C21 I29:I31 F29:F31 C29:C31 I40:I48 F40:F48 C40:C48" xr:uid="{4A0D4DC8-F6F9-4765-AB49-E4E0ACDB1361}">
@@ -5809,7 +5809,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6016,12 +6016,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6157,13 +6154,16 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F62C71A-5318-410B-8440-006B73523578}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F1A1E89-A0AE-4DED-85B2-2445C39C0F55}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6171,5 +6171,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F1A1E89-A0AE-4DED-85B2-2445C39C0F55}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F62C71A-5318-410B-8440-006B73523578}"/>
 </file>
</xml_diff>